<commit_message>
corrected conlist and Source bounds
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -414,10 +414,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>546.4480874316939</v>
       </c>
       <c r="D2">
-        <v>139.047619047619</v>
+        <v>124.024199843872</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -428,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>2380.952380952381</v>
+        <v>2371.194379391101</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -439,7 +439,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added basic Monte Carlo functionality
The simulation can now run properly, I think, but at the moment it will
only output the total system cost. More to come later.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,24 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Fuel Type</t>
-  </si>
-  <si>
-    <t>MJ by Fuel</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Total System Cost</t>
-  </si>
-  <si>
-    <t>crudeoil</t>
-  </si>
-  <si>
-    <t>hydrogen</t>
-  </si>
-  <si>
-    <t>biomass</t>
   </si>
 </sst>
 </file>
@@ -389,57 +374,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>546.448087431694</v>
-      </c>
-      <c r="D2">
-        <v>68.08315059240589</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2">
+        <v>76.94748099912351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>2315.449754633589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3">
+        <v>49.85114036113452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>102.0391570728407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>146.2408298477399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>97.04754572435553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="B7">
+        <v>164.7445278873959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>132.5892791210916</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>173.5750807781629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>138.6433161874834</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>109.5178694554061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Steven's changes, tenatively finished MC
After implementing Steven's changes, the Monte Carlo simulation
capabilties of this model appear to be functioning effectively. If I
understand correctly, now we just need to test with more data sets.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,9 +14,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Total System Cost</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>crudeoil</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>CrOilopex</t>
+  </si>
+  <si>
+    <t>H2opex</t>
+  </si>
+  <si>
+    <t>BMopex</t>
+  </si>
+  <si>
+    <t>Kilometersopex</t>
+  </si>
+  <si>
+    <t>Refineryopex</t>
+  </si>
+  <si>
+    <t>RefineryTotalEff</t>
+  </si>
+  <si>
+    <t>MtGopex</t>
+  </si>
+  <si>
+    <t>MtGTotalEff</t>
+  </si>
+  <si>
+    <t>Gtkmopex</t>
+  </si>
+  <si>
+    <t>GtkmTotalEff</t>
+  </si>
+  <si>
+    <t>B2gasopex</t>
+  </si>
+  <si>
+    <t>B2gasTotalEff</t>
+  </si>
+  <si>
+    <t>GasHubopex</t>
+  </si>
+  <si>
+    <t>KmHubopex</t>
   </si>
 </sst>
 </file>
@@ -374,95 +425,656 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>76.94748099912351</v>
+        <v>89.76330367398238</v>
+      </c>
+      <c r="C2">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D2">
+        <v>2515.565922971293</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.009593184099743147</v>
+      </c>
+      <c r="G2">
+        <v>0.03359924929753556</v>
+      </c>
+      <c r="H2">
+        <v>0.02712330684930081</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0.9083301713430862</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.8393132187520682</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0.3834792511278912</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0.5014963212342863</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>49.85114036113452</v>
+        <v>159.6121613960446</v>
+      </c>
+      <c r="C3">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D3">
+        <v>2340.066895963945</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.0240511167533359</v>
+      </c>
+      <c r="G3">
+        <v>0.06259200320222152</v>
+      </c>
+      <c r="H3">
+        <v>0.02921956733254961</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0.943031404594624</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0.8433247319912461</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0.4018074915740261</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0.4763978139591038</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>102.0391570728407</v>
+        <v>204.5351521568307</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2524.491274801826</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <v>0.03357751540721995</v>
+      </c>
+      <c r="G4">
+        <v>0.07549428810089714</v>
+      </c>
+      <c r="H4">
+        <v>0.0139504805487405</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0.8974002424928506</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0.8211517699504211</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.3937825643170712</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0.46648203908921</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>146.2408298477399</v>
+        <v>99.63469372619464</v>
+      </c>
+      <c r="C5">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D5">
+        <v>2277.865007796378</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.01170398372286112</v>
+      </c>
+      <c r="G5">
+        <v>0.04093266013849767</v>
+      </c>
+      <c r="H5">
+        <v>0.02512672877236114</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0.90784189705712</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0.8658110833546366</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0.4051389052843082</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0.5234251229582514</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>97.04754572435553</v>
+        <v>112.1981862574339</v>
+      </c>
+      <c r="C6">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D6">
+        <v>2240.579972867133</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.02178791405829147</v>
+      </c>
+      <c r="G6">
+        <v>0.04476172397578676</v>
+      </c>
+      <c r="H6">
+        <v>0.03410438942073959</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.9227786854325505</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.8360559476312721</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0.4206097321456089</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0.562761902784114</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>164.7445278873959</v>
+        <v>184.4413902559322</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2269.257107971565</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+      <c r="F7">
+        <v>0.007722111657192525</v>
+      </c>
+      <c r="G7">
+        <v>0.07891332862302258</v>
+      </c>
+      <c r="H7">
+        <v>0.005366758364442233</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0.9139686526111037</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0.8248050609430652</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0.4081453109215342</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0.5784130286983944</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:19">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>132.5892791210916</v>
+        <v>161.9737737281883</v>
+      </c>
+      <c r="C8">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D8">
+        <v>2135.45591735711</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.03221984957766327</v>
+      </c>
+      <c r="G8">
+        <v>0.06760490693144799</v>
+      </c>
+      <c r="H8">
+        <v>0.0346546501019294</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0.9023623865062289</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0.8542749271177579</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0.4315254083015325</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0.5660620628112978</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:19">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>173.5750807781629</v>
+        <v>171.504759153921</v>
+      </c>
+      <c r="C9">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D9">
+        <v>2297.450528203048</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.02612087647534168</v>
+      </c>
+      <c r="G9">
+        <v>0.0684371890631784</v>
+      </c>
+      <c r="H9">
+        <v>0.02630181878754293</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0.9056277005616411</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0.8147972161559413</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0.4225051920595571</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0.4609425690849009</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:19">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>138.6433161874834</v>
+        <v>183.4492149122224</v>
+      </c>
+      <c r="C10">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D10">
+        <v>2048.196463346483</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.007163787159909664</v>
+      </c>
+      <c r="G10">
+        <v>0.08765495904947818</v>
+      </c>
+      <c r="H10">
+        <v>0.05284505106210957</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0.9375961848594645</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0.815267884722407</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0.4582580865564485</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0.5536392857362011</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>109.5178694554061</v>
+        <v>178.1232256873284</v>
+      </c>
+      <c r="C11">
+        <v>546.448087431694</v>
+      </c>
+      <c r="D11">
+        <v>2340.2063569377</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.01644606849524194</v>
+      </c>
+      <c r="G11">
+        <v>0.07227409775677124</v>
+      </c>
+      <c r="H11">
+        <v>0.03149507711992676</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0.9453982591990508</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0.8375477934730711</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0.4037719175555546</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0.5401707860582325</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
put sinkDemand in outcolumns
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -40,6 +40,9 @@
     <t>Kilometersopex</t>
   </si>
   <si>
+    <t>KilometersDemand</t>
+  </si>
+  <si>
     <t>Refineryopex</t>
   </si>
   <si>
@@ -68,16 +71,13 @@
   </si>
   <si>
     <t>KmHubopex</t>
-  </si>
-  <si>
-    <t>KilometersDemand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +140,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -218,6 +223,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -252,6 +258,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,14 +434,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,624 +520,624 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>70.10661191017485</v>
+        <v>158.02588313103041</v>
       </c>
       <c r="C2">
-        <v>546.448087431694</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2160.481481104678</v>
+        <v>2481.1184299954439</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>999.99999999999977</v>
       </c>
       <c r="F2">
-        <v>0.0146697711719883</v>
+        <v>3.2201818214439272E-2</v>
       </c>
       <c r="G2">
-        <v>0.0287391232247146</v>
+        <v>6.2174504584578613E-2</v>
       </c>
       <c r="H2">
-        <v>0.01771822770231993</v>
+        <v>3.7635739303961552E-3</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>984.18666278232513</v>
       </c>
       <c r="K2">
-        <v>0.898482110537456</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.89814655704936708</v>
       </c>
       <c r="M2">
-        <v>0.8252649628029379</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.83774938188002668</v>
       </c>
       <c r="O2">
-        <v>0.4372181129518334</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>0.38659735225763159</v>
       </c>
       <c r="Q2">
-        <v>0.5866404293961521</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>0.46721126139023389</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
-        <v>994.2092860444217</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>79.22689102960678</v>
+        <v>110.3849719851686</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D3">
-        <v>3154.592854914126</v>
+        <v>2162.0139685574318</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.02837055954968281</v>
+        <v>6.8734653534395342E-3</v>
       </c>
       <c r="G3">
-        <v>0.02511477539999801</v>
+        <v>4.931928356591516E-2</v>
       </c>
       <c r="H3">
-        <v>0.01726372275010582</v>
+        <v>1.7064393788532108E-2</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>996.12709555098593</v>
       </c>
       <c r="K3">
-        <v>0.9425024312613505</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.91974331727384595</v>
       </c>
       <c r="M3">
-        <v>0.8466413585875031</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.83107966783797538</v>
       </c>
       <c r="O3">
-        <v>0.3757752103957357</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>0.43321215826018478</v>
       </c>
       <c r="Q3">
-        <v>0.49187075748033</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.52269482164210224</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3">
-        <v>1003.623731409744</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>191.7161782016296</v>
+        <v>124.3593793844814</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D4">
-        <v>2441.218348746741</v>
+        <v>2653.7813071409369</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.04397332062300463</v>
+        <v>1.7274492456431801E-2</v>
       </c>
       <c r="G4">
-        <v>0.07699149437548028</v>
+        <v>4.3304158376230473E-2</v>
       </c>
       <c r="H4">
-        <v>0.003763129434775726</v>
+        <v>3.768709715816157E-2</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1000.006194004161</v>
       </c>
       <c r="K4">
-        <v>0.8950289765673765</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.93284418641239586</v>
       </c>
       <c r="M4">
-        <v>0.8375408827080725</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.83092504235018483</v>
       </c>
       <c r="O4">
-        <v>0.3889842022029329</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>0.36834753518694208</v>
       </c>
       <c r="Q4">
-        <v>0.5345833474196523</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>0.5339359156569512</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <v>1003.269422811849</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>115.0333062499625</v>
+        <v>141.84372775527521</v>
       </c>
       <c r="C5">
-        <v>546.448087431694</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D5">
-        <v>2491.261454522022</v>
+        <v>2356.328596929176</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.03764343372184664</v>
+        <v>8.8068846397817476E-3</v>
       </c>
       <c r="G5">
-        <v>0.03791778808154903</v>
+        <v>5.8154547148567173E-2</v>
       </c>
       <c r="H5">
-        <v>0.02412984145219009</v>
+        <v>4.9943186974120819E-2</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>987.32632260977812</v>
       </c>
       <c r="K5">
-        <v>0.878805781733572</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>0.91400283819675132</v>
       </c>
       <c r="M5">
-        <v>0.8186341002493961</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.86377799808277245</v>
       </c>
       <c r="O5">
-        <v>0.3913411912680678</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>0.38950858494722301</v>
       </c>
       <c r="Q5">
-        <v>0.5161199717426285</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>0.50164226720664173</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5">
-        <v>986.0441310333435</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>122.8470698929063</v>
+        <v>145.7292557456382</v>
       </c>
       <c r="C6">
-        <v>546.448087431694</v>
+        <v>546.44808743169392</v>
       </c>
       <c r="D6">
-        <v>2256.460035069343</v>
+        <v>2609.7460073553252</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.003438876620532195</v>
+        <v>3.0102794227942719E-2</v>
       </c>
       <c r="G6">
-        <v>0.05360959221995949</v>
+        <v>4.9537250387227921E-2</v>
       </c>
       <c r="H6">
-        <v>0.04637188284100258</v>
+        <v>1.553751704643268E-2</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1000.017253009715</v>
       </c>
       <c r="K6">
-        <v>0.9408705042323471</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.9313166937594809</v>
       </c>
       <c r="M6">
-        <v>0.8285769919326229</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.86958509642500992</v>
       </c>
       <c r="O6">
-        <v>0.4029016142316865</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>0.35993692846630643</v>
       </c>
       <c r="Q6">
-        <v>0.4529930399159297</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>0.43833990872299428</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>960.4319348106823</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>159.4490488755924</v>
+        <v>127.8121957657857</v>
       </c>
       <c r="C7">
-        <v>546.448087431694</v>
+        <v>546.44808743169392</v>
       </c>
       <c r="D7">
-        <v>2464.227483210967</v>
+        <v>2304.9940745391709</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.01356197338627334</v>
+        <v>1.2059145277301499E-3</v>
       </c>
       <c r="G7">
-        <v>0.06169809219835226</v>
+        <v>5.5164231215615027E-2</v>
       </c>
       <c r="H7">
-        <v>0.037106438061745</v>
+        <v>2.393140519025732E-2</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>989.65705825662656</v>
       </c>
       <c r="K7">
-        <v>0.9012697027685009</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.92669351628895547</v>
       </c>
       <c r="M7">
-        <v>0.8380057870548839</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>0.83749787889039473</v>
       </c>
       <c r="O7">
-        <v>0.3900177158839919</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>0.40612685964624717</v>
       </c>
       <c r="Q7">
-        <v>0.3680741043713345</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>0.59679578345618634</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7">
-        <v>997.4835677620939</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>160.491790011684</v>
+        <v>156.13050815920991</v>
       </c>
       <c r="C8">
-        <v>546.448087431694</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D8">
-        <v>2602.541797657739</v>
+        <v>2740.8561600601529</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.01057115975040145</v>
+        <v>7.3628105298367934E-3</v>
       </c>
       <c r="G8">
-        <v>0.05944772918666832</v>
+        <v>5.549620466902587E-2</v>
       </c>
       <c r="H8">
-        <v>0.01834855202294131</v>
+        <v>1.897901985493813E-2</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>986.80915201166783</v>
       </c>
       <c r="K8">
-        <v>0.9305093065369203</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.941356053461611</v>
       </c>
       <c r="M8">
-        <v>0.8468116294527408</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>0.83029750692830862</v>
       </c>
       <c r="O8">
-        <v>0.3644894726020976</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>0.35367877855158369</v>
       </c>
       <c r="Q8">
-        <v>0.5018796285136933</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>0.46571993186049199</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8">
-        <v>988.6185346163203</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>118.7740385122494</v>
+        <v>83.146185300306243</v>
       </c>
       <c r="C9">
-        <v>546.448087431694</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D9">
-        <v>2083.32141899004</v>
+        <v>2908.2686214788132</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.02262723273214044</v>
+        <v>5.8373519168102234E-3</v>
       </c>
       <c r="G9">
-        <v>0.05107681872415298</v>
+        <v>2.7492775226878079E-2</v>
       </c>
       <c r="H9">
-        <v>0.023017050732101</v>
+        <v>3.5621610521512949E-2</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>999.77371592987447</v>
       </c>
       <c r="K9">
-        <v>0.9400745853639163</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.94121767564033554</v>
       </c>
       <c r="M9">
-        <v>0.847086054733817</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.8556829790046292</v>
       </c>
       <c r="O9">
-        <v>0.4185477502696664</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>0.33293800111208371</v>
       </c>
       <c r="Q9">
-        <v>0.562822020835404</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>0.51779287579049083</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9">
-        <v>953.641997018118</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>151.5955164858706</v>
+        <v>131.61946893487499</v>
       </c>
       <c r="C10">
-        <v>546.4480874316939</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D10">
-        <v>2365.188086051659</v>
+        <v>2441.1348789787298</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.03489716639716593</v>
+        <v>2.6492232501088338E-3</v>
       </c>
       <c r="G10">
-        <v>0.0560319187437591</v>
+        <v>5.3324298906061267E-2</v>
       </c>
       <c r="H10">
-        <v>0.01759935038891854</v>
+        <v>2.3074266546190041E-2</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>990.80670025482425</v>
       </c>
       <c r="K10">
-        <v>0.9289774887010676</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>0.90428607900954106</v>
       </c>
       <c r="M10">
-        <v>0.8304387518272505</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.84200792976332195</v>
       </c>
       <c r="O10">
-        <v>0.4215582271372024</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>0.38861255660112992</v>
       </c>
       <c r="Q10">
-        <v>0.442027644658124</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>0.56568343834328805</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10">
-        <v>1041.999959373587</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>197.9227901979066</v>
+        <v>73.628174704552976</v>
       </c>
       <c r="C11">
-        <v>546.4480874316939</v>
+        <v>546.44808743169403</v>
       </c>
       <c r="D11">
-        <v>2558.140953031314</v>
+        <v>2643.581028045432</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.007164692656490319</v>
+        <v>2.9834028847180831E-3</v>
       </c>
       <c r="G11">
-        <v>0.07583931501852498</v>
+        <v>2.7234988880743029E-2</v>
       </c>
       <c r="H11">
-        <v>0.03005382725445438</v>
+        <v>1.989741273540744E-2</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>992.58330459650449</v>
       </c>
       <c r="K11">
-        <v>0.9166782033311098</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.9143952679391637</v>
       </c>
       <c r="M11">
-        <v>0.8218428143829135</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>0.83867069539297923</v>
       </c>
       <c r="O11">
-        <v>0.3799333758929527</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>0.36535506689531411</v>
       </c>
       <c r="Q11">
-        <v>0.4992296965279395</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>0.54700949288064826</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
-        <v>989.0831453509775</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is a test
I want to make sure I properly understand how git handles commits on a
branch. You can ignore this commit.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -546,49 +546,49 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>195.0069102805903</v>
+        <v>121.7744789210046</v>
       </c>
       <c r="C2">
-        <v>16.37240170114682</v>
+        <v>40</v>
       </c>
       <c r="D2">
-        <v>223.6666899063773</v>
+        <v>212.815665118663</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3046.395281440311</v>
+        <v>2102.493658644074</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>610.5473328328467</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.02452288890473963</v>
+        <v>0.002348093274886724</v>
       </c>
       <c r="K2">
-        <v>0.06221187317580171</v>
+        <v>0.05205780726319665</v>
       </c>
       <c r="L2">
-        <v>0.06004362877703256</v>
+        <v>0.01936550632414199</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1001.546187016945</v>
+        <v>1011.226663093531</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.8941876865246061</v>
+        <v>0.93978044280003</v>
       </c>
       <c r="Q2">
         <v>200</v>
@@ -597,28 +597,28 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0.8296150187497769</v>
+        <v>0.8275679403271208</v>
       </c>
       <c r="T2">
-        <v>2527.335278531336</v>
+        <v>1739.956346634909</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.3672251794272522</v>
+        <v>0.4429960375016347</v>
       </c>
       <c r="W2">
-        <v>1001.546187016945</v>
+        <v>1011.226663093531</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>0.4767301622731319</v>
+        <v>0.5613696935541674</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>342.7427691326894</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -632,49 +632,49 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>114.0607491686329</v>
+        <v>210.6375000841791</v>
       </c>
       <c r="C3">
-        <v>15.55963215570908</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>212.5632808156979</v>
+        <v>216.8082181648471</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>2997.150922555896</v>
+        <v>2406.135090620478</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>603.2409607583298</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.00526963314993755</v>
+        <v>0.02220982661171617</v>
       </c>
       <c r="K3">
-        <v>0.03768265982457567</v>
+        <v>0.08055904135278205</v>
       </c>
       <c r="L3">
-        <v>0.02434972138313655</v>
+        <v>0.01986982261615612</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>996.9122513350209</v>
+        <v>994.5797031875584</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.9408962791339733</v>
+        <v>0.9224742571701446</v>
       </c>
       <c r="Q3">
         <v>200</v>
@@ -683,28 +683,28 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0.8157821215605918</v>
+        <v>0.8330705843437558</v>
       </c>
       <c r="T3">
-        <v>2445.022138239934</v>
+        <v>2004.480365953217</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0.3769012882434292</v>
+        <v>0.3932621536389742</v>
       </c>
       <c r="W3">
-        <v>996.9122513350209</v>
+        <v>994.5797031875584</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>0.4460531942133563</v>
+        <v>0.5380433214428376</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>324.5697701567802</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -718,49 +718,49 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>141.8694817229864</v>
+        <v>99.04886500521728</v>
       </c>
       <c r="C4">
         <v>40</v>
       </c>
       <c r="D4">
-        <v>212.352668818627</v>
+        <v>216.9987957756236</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>2430.081564951446</v>
+        <v>1941.622773228155</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>611.3946160619125</v>
+        <v>602.8922037306088</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.0257223262103678</v>
+        <v>0.0113203468964704</v>
       </c>
       <c r="K4">
-        <v>0.05169881595332022</v>
+        <v>0.04469268339914839</v>
       </c>
       <c r="L4">
-        <v>0.01762354008841846</v>
+        <v>0.01628156976606811</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>974.7074151959887</v>
+        <v>1008.049311634372</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9418294628113313</v>
+        <v>0.9216641008773141</v>
       </c>
       <c r="Q4">
         <v>200</v>
@@ -769,28 +769,28 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.8209452698122482</v>
+        <v>0.8433294465746841</v>
       </c>
       <c r="T4">
-        <v>1994.963966004835</v>
+        <v>1637.427658803304</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4">
-        <v>0.3981169233047824</v>
+        <v>0.4798330029566718</v>
       </c>
       <c r="W4">
-        <v>974.7074151959887</v>
+        <v>1008.049311634372</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>0.414348410058319</v>
+        <v>0.4369039344566191</v>
       </c>
       <c r="Z4">
-        <v>253.3303870834698</v>
+        <v>263.4059758631246</v>
       </c>
       <c r="AA4">
         <v>0</v>
@@ -804,49 +804,49 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>150.8817711372159</v>
+        <v>94.44367166706512</v>
       </c>
       <c r="C5">
-        <v>40.00000000000001</v>
+        <v>16.09663463598934</v>
       </c>
       <c r="D5">
-        <v>217.3042912822645</v>
+        <v>219.8993802730784</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2508.232377046967</v>
+        <v>2853.159315040723</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>602.333146953456</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.004488578146070251</v>
+        <v>0.008552758480979165</v>
       </c>
       <c r="K5">
-        <v>0.05323732373615354</v>
+        <v>0.03244225616477758</v>
       </c>
       <c r="L5">
-        <v>0.02718562786190657</v>
+        <v>0.03804039643536632</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1006.086638669547</v>
+        <v>1013.306053125703</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.920368386743972</v>
+        <v>0.9095068833374305</v>
       </c>
       <c r="Q5">
         <v>200</v>
@@ -855,28 +855,28 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0.8251549975806217</v>
+        <v>0.840365493926777</v>
       </c>
       <c r="T5">
-        <v>2069.680481013827</v>
+        <v>2397.696637035982</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0.3931873223339269</v>
+        <v>0.3900786714964157</v>
       </c>
       <c r="W5">
-        <v>1006.086638669547</v>
+        <v>1013.306053125703</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>0.4799947824479487</v>
+        <v>0.5162579709204294</v>
       </c>
       <c r="Z5">
-        <v>289.1167678331124</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -890,49 +890,49 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>206.0151730223007</v>
+        <v>131.3991036849226</v>
       </c>
       <c r="C6">
-        <v>40.00000000000001</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>217.1579832821567</v>
+        <v>216.4676429633167</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2736.594889309589</v>
+        <v>2482.269757635597</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>602.6008905936533</v>
+        <v>603.8642133771305</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.02448315454606691</v>
+        <v>0.02171922704753687</v>
       </c>
       <c r="K6">
-        <v>0.06858679466424583</v>
+        <v>0.04876516460272357</v>
       </c>
       <c r="L6">
-        <v>0.02158010219928313</v>
+        <v>0.009355249664325332</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1023.739735273847</v>
+        <v>988.7071353895649</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.9209884756580047</v>
+        <v>0.9239256142955861</v>
       </c>
       <c r="Q6">
         <v>200</v>
@@ -941,28 +941,28 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0.8519370354569534</v>
+        <v>0.8337761221893575</v>
       </c>
       <c r="T6">
-        <v>2331.406537245061</v>
+        <v>2069.657252749324</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0.3578591399661504</v>
+        <v>0.3904080811222203</v>
       </c>
       <c r="W6">
-        <v>1023.739735273847</v>
+        <v>988.7071353895649</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0.5465097415581022</v>
+        <v>0.4352623232209656</v>
       </c>
       <c r="Z6">
-        <v>329.3272569810197</v>
+        <v>262.8393404245307</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -976,79 +976,79 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>210.3943289132366</v>
+        <v>132.6946672458907</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>40.00000000000001</v>
       </c>
       <c r="D7">
-        <v>210.8931742376801</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>2524.48167866078</v>
+        <v>2148.750086759504</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>614.0654911450455</v>
+        <v>1000</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.03039519206980118</v>
+        <v>0.01038766567243881</v>
       </c>
       <c r="K7">
-        <v>0.075024350053667</v>
+        <v>0.05864246512268719</v>
       </c>
       <c r="L7">
-        <v>0.02375413277980732</v>
+        <v>0.006686665225725419</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>1020.5778852583</v>
+        <v>1015.651705141702</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0.9483474309822694</v>
+        <v>0.9414457470998366</v>
       </c>
       <c r="Q7">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0.8620282240290101</v>
+        <v>0.8287895735837484</v>
       </c>
       <c r="T7">
-        <v>2176.174458049726</v>
+        <v>1780.861668143451</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0.3882416450517856</v>
+        <v>0.4385542201385005</v>
       </c>
       <c r="W7">
-        <v>1020.5778852583</v>
+        <v>1015.651705141702</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>0.4112651881553938</v>
+        <v>0.5350474224610067</v>
       </c>
       <c r="Z7">
-        <v>252.5437597555014</v>
+        <v>535.0474224610067</v>
       </c>
       <c r="AA7">
         <v>0</v>
@@ -1062,49 +1062,49 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>135.7438825309016</v>
+        <v>84.26707576041001</v>
       </c>
       <c r="C8">
-        <v>40.00000000000001</v>
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>225.9532802531134</v>
+        <v>215.0116188266796</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2263.920682801419</v>
+        <v>1932.703289267768</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>586.5054971368027</v>
+        <v>606.5287375471762</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.01834521704604285</v>
+        <v>0.02160526545129312</v>
       </c>
       <c r="K8">
-        <v>0.05343249263847207</v>
+        <v>0.03613067964798337</v>
       </c>
       <c r="L8">
-        <v>0.01812735839037085</v>
+        <v>0.01614401537016744</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1012.381961101153</v>
+        <v>990.6938417686193</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0.8851387321129374</v>
+        <v>0.930182290107864</v>
       </c>
       <c r="Q8">
         <v>200</v>
@@ -1113,28 +1113,28 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>0.8470047133927943</v>
+        <v>0.8602370220641031</v>
       </c>
       <c r="T8">
-        <v>1917.551489080235</v>
+        <v>1662.582922093202</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0.4166699619360318</v>
+        <v>0.451632929765607</v>
       </c>
       <c r="W8">
-        <v>1012.381961101153</v>
+        <v>990.6938417686193</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>0.5322132588149023</v>
+        <v>0.5457268637451181</v>
       </c>
       <c r="Z8">
-        <v>312.1460019440321</v>
+        <v>330.9990257129064</v>
       </c>
       <c r="AA8">
         <v>0</v>
@@ -1148,79 +1148,79 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>112.0608846513275</v>
+        <v>95.81084823624377</v>
       </c>
       <c r="C9">
         <v>40</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>219.5232869633142</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>2064.293057906641</v>
+        <v>2235.171936789313</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>598.2723848571351</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.02297127951841579</v>
+        <v>0.00310669693234989</v>
       </c>
       <c r="K9">
-        <v>0.05276057339089033</v>
+        <v>0.04007753794520412</v>
       </c>
       <c r="L9">
-        <v>0.003147599269338761</v>
+        <v>0.009274484237896724</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>1016.571325306001</v>
+        <v>989.6338231384073</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0.9015562974029467</v>
+        <v>0.911065075448798</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9">
-        <v>0.8578027257244812</v>
+        <v>0.8480620151444597</v>
       </c>
       <c r="T9">
-        <v>1770.756211766441</v>
+        <v>1895.56441690789</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9">
-        <v>0.4354257695562926</v>
+        <v>0.4102260702268819</v>
       </c>
       <c r="W9">
-        <v>1016.571325306001</v>
+        <v>989.6338231384073</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>0.5639042433138978</v>
+        <v>0.5296023049271085</v>
       </c>
       <c r="Z9">
-        <v>563.9042433138977</v>
+        <v>316.8464339945768</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -1234,49 +1234,49 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>131.3777617639103</v>
+        <v>165.5847935824491</v>
       </c>
       <c r="C10">
-        <v>16.33907086210717</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>223.2113505752345</v>
+        <v>217.9593461984611</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>2601.679498268624</v>
+        <v>2550.877625225707</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>601.1343964568161</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.02856099409530397</v>
+        <v>0.03112316767652012</v>
       </c>
       <c r="K10">
-        <v>0.04804689577686777</v>
+        <v>0.05450283808351926</v>
       </c>
       <c r="L10">
-        <v>0.03233245612175138</v>
+        <v>0.03288971358490739</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1002.420838364033</v>
+        <v>983.6246111427911</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>0.8960117820378897</v>
+        <v>0.9176023120288297</v>
       </c>
       <c r="Q10">
         <v>200</v>
@@ -1285,28 +1285,28 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0.8420504339628174</v>
+        <v>0.843787696727783</v>
       </c>
       <c r="T10">
-        <v>2190.74535054926</v>
+        <v>2152.399156023636</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10">
-        <v>0.4192921835584589</v>
+        <v>0.3645456662837667</v>
       </c>
       <c r="W10">
-        <v>1002.420838364033</v>
+        <v>983.6246111427911</v>
       </c>
       <c r="X10">
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>0.4832423747172801</v>
+        <v>0.5752813416454232</v>
       </c>
       <c r="Z10">
-        <v>0</v>
+        <v>345.821402102889</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -1320,79 +1320,79 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>157.207514328091</v>
+        <v>87.87486582850033</v>
       </c>
       <c r="C11">
         <v>40</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>224.2148775141743</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>2114.213088858497</v>
+        <v>2640.103597130349</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1000</v>
+        <v>589.6867741490611</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.02625684770907999</v>
+        <v>0.02329551994717612</v>
       </c>
       <c r="K11">
-        <v>0.06612645055040436</v>
+        <v>0.0286362862600064</v>
       </c>
       <c r="L11">
-        <v>0.01740210705467193</v>
+        <v>0.01195363644299093</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>1030.005553117358</v>
+        <v>983.9256373026786</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0.9388372227906356</v>
+        <v>0.8920014684902277</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.8475389390374807</v>
+        <v>0.8449113856185803</v>
       </c>
       <c r="T11">
-        <v>1791.877918230285</v>
+        <v>2230.653588428001</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11">
-        <v>0.4375480352361826</v>
+        <v>0.3644502356478774</v>
       </c>
       <c r="W11">
-        <v>1030.005553117358</v>
+        <v>983.9256373026786</v>
       </c>
       <c r="X11">
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>0.5621620274899031</v>
+        <v>0.4563430603566268</v>
       </c>
       <c r="Z11">
-        <v>562.162027489903</v>
+        <v>269.0994671670095</v>
       </c>
       <c r="AA11">
         <v>0</v>

</xml_diff>

<commit_message>
Added some comments on pyomo constraints.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>52.6452763328954</v>
+        <v>53.6140288729115</v>
       </c>
       <c r="C2">
         <v>87.214</v>
@@ -672,130 +672,130 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>371.5458029604555</v>
+        <v>428.280244309893</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>492.5150211550128</v>
+        <v>464.0518752201003</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.01338088601337492</v>
+        <v>0.0121570441834635</v>
       </c>
       <c r="K2">
-        <v>0.02327182389671468</v>
+        <v>0.01963277841345167</v>
       </c>
       <c r="L2">
-        <v>0.0470816290870748</v>
+        <v>0.05575837250302004</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>856.5423098386788</v>
+        <v>882.1481460203819</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>8.353174356277631</v>
+        <v>7.338232931159531</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>22.44291380449058</v>
+        <v>23.81406428126117</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
-        <v>130.6370847869817</v>
+        <v>133.3838248188448</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>416.9472149149414</v>
+        <v>407.8053181776484</v>
       </c>
       <c r="W2">
-        <v>0.001017039800894917</v>
+        <v>0.001003988479294612</v>
       </c>
       <c r="X2">
-        <v>0.934871712898634</v>
+        <v>0.9335099068773931</v>
       </c>
       <c r="Y2">
-        <v>1113.851114327069</v>
+        <v>1112.228593147609</v>
       </c>
       <c r="Z2">
-        <v>0.0009937020174443675</v>
+        <v>0.001019120703483518</v>
       </c>
       <c r="AA2">
-        <v>0.5298609988206074</v>
+        <v>0.5188767414771587</v>
       </c>
       <c r="AB2">
-        <v>196.8676302642316</v>
+        <v>222.2246576065587</v>
       </c>
       <c r="AC2">
-        <v>0.0009663204047517917</v>
+        <v>0.0009774128254531375</v>
       </c>
       <c r="AD2">
-        <v>0.837034118047576</v>
+        <v>0.8397498655111978</v>
       </c>
       <c r="AE2">
-        <v>412.2518763576695</v>
+        <v>389.6874998062983</v>
       </c>
       <c r="AF2">
-        <v>0.0009918508121129147</v>
+        <v>0.000984614700336758</v>
       </c>
       <c r="AG2">
-        <v>0.7647703094927919</v>
+        <v>0.7657197407816889</v>
       </c>
       <c r="AH2">
-        <v>856.5423098386788</v>
+        <v>882.1481460203819</v>
       </c>
       <c r="AI2">
-        <v>0.0009545230705377617</v>
+        <v>0.0009619134810018753</v>
       </c>
       <c r="AJ2">
-        <v>0.08561599683653895</v>
+        <v>0.08800686901942845</v>
       </c>
       <c r="AK2">
-        <v>8.353174356277631</v>
+        <v>7.338232931159531</v>
       </c>
       <c r="AL2">
-        <v>0.0009754904562939866</v>
+        <v>0.001027975283699864</v>
       </c>
       <c r="AM2">
-        <v>0.6526911333532717</v>
+        <v>0.6729757209362213</v>
       </c>
       <c r="AN2">
-        <v>22.44291380449058</v>
+        <v>23.81406428126117</v>
       </c>
       <c r="AO2">
-        <v>0.00102442440299449</v>
+        <v>0.0009916803794674416</v>
       </c>
       <c r="AP2">
-        <v>0.6528109389653927</v>
+        <v>0.7090897307023841</v>
       </c>
       <c r="AQ2">
-        <v>130.6370847869817</v>
+        <v>133.3838248188448</v>
       </c>
       <c r="AR2">
-        <v>0.0009764494888525672</v>
+        <v>0.001019279789329731</v>
       </c>
       <c r="AS2">
-        <v>1.539086252855079</v>
+        <v>1.537638227593586</v>
       </c>
       <c r="AT2">
-        <v>416.9472149149414</v>
+        <v>407.8053181776484</v>
       </c>
       <c r="AU2">
-        <v>0.0009985527904082332</v>
+        <v>0.0009711228535752979</v>
       </c>
     </row>
     <row r="3" spans="1:47">
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>41.825256347505</v>
+        <v>50.88869313145803</v>
       </c>
       <c r="C3">
         <v>87.214</v>
@@ -815,130 +815,130 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>495.2171634340177</v>
+        <v>373.8942591027078</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>159.9061137940548</v>
+        <v>483.1272158022734</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.01375598170256241</v>
+        <v>0.01294994174673858</v>
       </c>
       <c r="K3">
-        <v>0.02684075058011019</v>
+        <v>0.01726884304971958</v>
       </c>
       <c r="L3">
-        <v>0.0481346617520567</v>
+        <v>0.05002139632559284</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>745.7284796816422</v>
+        <v>877.7339717510523</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>7.577780469740994</v>
+        <v>8.721962734239312</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>23.60436130586512</v>
+        <v>22.0802847503616</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3">
-        <v>140.7171086942494</v>
+        <v>140.4775773343349</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3">
-        <v>428.6296385041169</v>
+        <v>385.3970541968857</v>
       </c>
       <c r="W3">
-        <v>0.001005104783421494</v>
+        <v>0.000995149774882839</v>
       </c>
       <c r="X3">
-        <v>0.9371767525651296</v>
+        <v>0.928976817521297</v>
       </c>
       <c r="Y3">
-        <v>1116.59744942917</v>
+        <v>1106.827652504131</v>
       </c>
       <c r="Z3">
-        <v>0.0009991754024899742</v>
+        <v>0.001020713015940025</v>
       </c>
       <c r="AA3">
-        <v>0.5598874238173894</v>
+        <v>0.5092932733517126</v>
       </c>
       <c r="AB3">
-        <v>277.2658618652273</v>
+        <v>190.4218311058314</v>
       </c>
       <c r="AC3">
-        <v>0.0009983149207037972</v>
+        <v>0.0009677945558486553</v>
       </c>
       <c r="AD3">
-        <v>0.83170735319061</v>
+        <v>0.8526343593606128</v>
       </c>
       <c r="AE3">
-        <v>132.9950906626498</v>
+        <v>411.9308641352479</v>
       </c>
       <c r="AF3">
-        <v>0.001011469731547477</v>
+        <v>0.001021326573182564</v>
       </c>
       <c r="AG3">
-        <v>0.8028907824126361</v>
+        <v>0.780097536779125</v>
       </c>
       <c r="AH3">
-        <v>745.7284796816422</v>
+        <v>877.7339717510523</v>
       </c>
       <c r="AI3">
-        <v>0.0009891634874082136</v>
+        <v>0.001009066623769285</v>
       </c>
       <c r="AJ3">
-        <v>0.09227513370363367</v>
+        <v>0.09066699151633288</v>
       </c>
       <c r="AK3">
-        <v>7.577780469740994</v>
+        <v>8.721962734239312</v>
       </c>
       <c r="AL3">
-        <v>0.0009832618667035737</v>
+        <v>0.0009397195307849035</v>
       </c>
       <c r="AM3">
-        <v>0.6192274534539852</v>
+        <v>0.6659634939707622</v>
       </c>
       <c r="AN3">
-        <v>23.60436130586512</v>
+        <v>22.0802847503616</v>
       </c>
       <c r="AO3">
-        <v>0.001056819579634105</v>
+        <v>0.001014277797518422</v>
       </c>
       <c r="AP3">
-        <v>0.7205920383105378</v>
+        <v>0.6928431927694515</v>
       </c>
       <c r="AQ3">
-        <v>140.7171086942494</v>
+        <v>140.4775773343349</v>
       </c>
       <c r="AR3">
-        <v>0.001036481649388675</v>
+        <v>0.0009832926944251421</v>
       </c>
       <c r="AS3">
-        <v>1.517093015717739</v>
+        <v>1.529883474444269</v>
       </c>
       <c r="AT3">
-        <v>428.6296385041169</v>
+        <v>385.3970541968857</v>
       </c>
       <c r="AU3">
-        <v>0.001006392911927274</v>
+        <v>0.0009912096592654132</v>
       </c>
     </row>
     <row r="4" spans="1:47">
@@ -946,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>58.14781008274321</v>
+        <v>47.46779545447417</v>
       </c>
       <c r="C4">
         <v>87.214</v>
@@ -958,130 +958,130 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>458.0437306829778</v>
+        <v>341.0687738763023</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>558.3650423680397</v>
+        <v>472.0001521246543</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.01308218258930357</v>
+        <v>0.0115300034651086</v>
       </c>
       <c r="K4">
-        <v>0.0184365448458151</v>
+        <v>0.02053180538848691</v>
       </c>
       <c r="L4">
-        <v>0.05183212648653581</v>
+        <v>0.04657771966677064</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>976.6607944267188</v>
+        <v>900.6976035444858</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>7.191664607325146</v>
+        <v>7.667380358118211</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>21.13106636160556</v>
+        <v>26.1578000355324</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <v>136.2781353834299</v>
+        <v>133.5660467908301</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4">
-        <v>407.2672526405244</v>
+        <v>439.5063420473402</v>
       </c>
       <c r="W4">
-        <v>0.001010670228622558</v>
+        <v>0.0009868792904625199</v>
       </c>
       <c r="X4">
-        <v>0.9358650654674673</v>
+        <v>0.9329289269522153</v>
       </c>
       <c r="Y4">
-        <v>1115.034642345351</v>
+        <v>1111.536385726919</v>
       </c>
       <c r="Z4">
-        <v>0.0009937282985247385</v>
+        <v>0.00103041549829562</v>
       </c>
       <c r="AA4">
-        <v>0.5288905790651945</v>
+        <v>0.5749244562604591</v>
       </c>
       <c r="AB4">
-        <v>242.2550139581021</v>
+        <v>196.0887793682546</v>
       </c>
       <c r="AC4">
-        <v>0.001016168586085043</v>
+        <v>0.0009662965065815141</v>
       </c>
       <c r="AD4">
-        <v>0.8400033462225753</v>
+        <v>0.8317384541321819</v>
       </c>
       <c r="AE4">
-        <v>469.0285040028634</v>
+        <v>392.5806768783148</v>
       </c>
       <c r="AF4">
-        <v>0.0009600450533381133</v>
+        <v>0.0009663712199169086</v>
       </c>
       <c r="AG4">
-        <v>0.7768051132169992</v>
+        <v>0.8156074511419156</v>
       </c>
       <c r="AH4">
-        <v>976.6607944267188</v>
+        <v>900.6976035444858</v>
       </c>
       <c r="AI4">
-        <v>0.001054068779448436</v>
+        <v>0.0009943414030698786</v>
       </c>
       <c r="AJ4">
-        <v>0.08553370084399534</v>
+        <v>0.08992267946509611</v>
       </c>
       <c r="AK4">
-        <v>7.191664607325146</v>
+        <v>7.667380358118211</v>
       </c>
       <c r="AL4">
-        <v>0.001059594636644141</v>
+        <v>0.001013396974702585</v>
       </c>
       <c r="AM4">
-        <v>0.6892368721087813</v>
+        <v>0.6884004743780061</v>
       </c>
       <c r="AN4">
-        <v>21.13106636160556</v>
+        <v>26.1578000355324</v>
       </c>
       <c r="AO4">
-        <v>0.000947798115167675</v>
+        <v>0.001054883068875319</v>
       </c>
       <c r="AP4">
-        <v>0.7227400465033993</v>
+        <v>0.717093321352955</v>
       </c>
       <c r="AQ4">
-        <v>136.2781353834299</v>
+        <v>133.5660467908301</v>
       </c>
       <c r="AR4">
-        <v>0.0009685228243066268</v>
+        <v>0.0009527918609884159</v>
       </c>
       <c r="AS4">
-        <v>1.532560809857316</v>
+        <v>1.534836472662366</v>
       </c>
       <c r="AT4">
-        <v>407.2672526405244</v>
+        <v>439.5063420473402</v>
       </c>
       <c r="AU4">
-        <v>0.001007259509433724</v>
+        <v>0.0009412959238030525</v>
       </c>
     </row>
     <row r="5" spans="1:47">
@@ -1089,7 +1089,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>54.13863673039128</v>
+        <v>43.7977498963502</v>
       </c>
       <c r="C5">
         <v>87.214</v>
@@ -1101,130 +1101,130 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>390.7452911208738</v>
+        <v>415.4700470356821</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>453.2930913209966</v>
+        <v>345.3576008003247</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.01413906269423757</v>
+        <v>0.01103010409214692</v>
       </c>
       <c r="K5">
-        <v>0.01552008896158125</v>
+        <v>0.02212213483228839</v>
       </c>
       <c r="L5">
-        <v>0.05785043176715923</v>
+        <v>0.04847325101227368</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>891.3313380947036</v>
+        <v>864.0707544129565</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>7.80520956220842</v>
+        <v>7.588606235337236</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
-        <v>25.16430276162719</v>
+        <v>27.16178431793838</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5">
-        <v>142.7082776307537</v>
+        <v>131.8048820489254</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
-        <v>421.5174137883042</v>
+        <v>394.4487143788305</v>
       </c>
       <c r="W5">
-        <v>0.001039708942867721</v>
+        <v>0.001009354222655065</v>
       </c>
       <c r="X5">
-        <v>0.9270999768035113</v>
+        <v>0.9360264667164867</v>
       </c>
       <c r="Y5">
-        <v>1104.591494220511</v>
+        <v>1115.226943554804</v>
       </c>
       <c r="Z5">
-        <v>0.0009897817830112634</v>
+        <v>0.001016562264295554</v>
       </c>
       <c r="AA5">
-        <v>0.5859297898519683</v>
+        <v>0.5245048350321246</v>
       </c>
       <c r="AB5">
-        <v>228.9493063120998</v>
+        <v>217.9160484812395</v>
       </c>
       <c r="AC5">
-        <v>0.001028118559143242</v>
+        <v>0.001043291660256918</v>
       </c>
       <c r="AD5">
-        <v>0.8241534343406447</v>
+        <v>0.8334473952017766</v>
       </c>
       <c r="AE5">
-        <v>373.5830579750868</v>
+        <v>287.8373928001656</v>
       </c>
       <c r="AF5">
-        <v>0.000994146861664858</v>
+        <v>0.000964526567163855</v>
       </c>
       <c r="AG5">
-        <v>0.8162459771315652</v>
+        <v>0.8232497936962005</v>
       </c>
       <c r="AH5">
-        <v>891.3313380947036</v>
+        <v>864.0707544129565</v>
       </c>
       <c r="AI5">
-        <v>0.000948547922755406</v>
+        <v>0.001074578843016275</v>
       </c>
       <c r="AJ5">
-        <v>0.08958465923593556</v>
+        <v>0.09049085758354249</v>
       </c>
       <c r="AK5">
-        <v>7.80520956220842</v>
+        <v>7.588606235337236</v>
       </c>
       <c r="AL5">
-        <v>0.0009898832054743292</v>
+        <v>0.001033535304020922</v>
       </c>
       <c r="AM5">
-        <v>0.6678760880747846</v>
+        <v>0.6973004115240369</v>
       </c>
       <c r="AN5">
-        <v>25.16430276162719</v>
+        <v>27.16178431793838</v>
       </c>
       <c r="AO5">
-        <v>0.0009743489007912459</v>
+        <v>0.001083421801540355</v>
       </c>
       <c r="AP5">
-        <v>0.6735523254151664</v>
+        <v>0.7107488884166304</v>
       </c>
       <c r="AQ5">
-        <v>142.7082776307537</v>
+        <v>131.8048820489254</v>
       </c>
       <c r="AR5">
-        <v>0.001055794534799191</v>
+        <v>0.0009826820003566745</v>
       </c>
       <c r="AS5">
-        <v>1.51376447916093</v>
+        <v>1.499024615495767</v>
       </c>
       <c r="AT5">
-        <v>421.5174137883042</v>
+        <v>394.4487143788305</v>
       </c>
       <c r="AU5">
-        <v>0.001021257233736316</v>
+        <v>0.001034384163985833</v>
       </c>
     </row>
     <row r="6" spans="1:47">
@@ -1232,7 +1232,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>53.04784157184913</v>
+        <v>38.8269351033933</v>
       </c>
       <c r="C6">
         <v>87.214</v>
@@ -1244,130 +1244,130 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>406.0828522221991</v>
+        <v>477.338853621536</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>520.2202068062979</v>
+        <v>250.9276648657085</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.01282078960207512</v>
+        <v>0.01178108171379331</v>
       </c>
       <c r="K6">
-        <v>0.01847199926764121</v>
+        <v>0.01805600182762122</v>
       </c>
       <c r="L6">
-        <v>0.04833631808869387</v>
+        <v>0.04658715462149561</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>884.8169753298216</v>
+        <v>843.49852971526</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>8.737289720709475</v>
+        <v>6.717572957623268</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
-        <v>24.49978526467693</v>
+        <v>24.38596837934758</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>124.103253809559</v>
+        <v>125.5822890087317</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6">
-        <v>427.719890611368</v>
+        <v>389.736586751124</v>
       </c>
       <c r="W6">
-        <v>0.001002251269835089</v>
+        <v>0.001001448769775207</v>
       </c>
       <c r="X6">
-        <v>0.9364929139280332</v>
+        <v>0.9349002828449477</v>
       </c>
       <c r="Y6">
-        <v>1115.782691192889</v>
+        <v>1113.885153934963</v>
       </c>
       <c r="Z6">
-        <v>0.001019702997814731</v>
+        <v>0.0009997576004930654</v>
       </c>
       <c r="AA6">
-        <v>0.5750424759543209</v>
+        <v>0.5014827540465786</v>
       </c>
       <c r="AB6">
-        <v>233.514888784446</v>
+        <v>239.3772029275645</v>
       </c>
       <c r="AC6">
-        <v>0.001006377950827654</v>
+        <v>0.0009686568999787306</v>
       </c>
       <c r="AD6">
-        <v>0.838539647122</v>
+        <v>0.8471286151264793</v>
       </c>
       <c r="AE6">
-        <v>436.2252686410868</v>
+        <v>212.568005234609</v>
       </c>
       <c r="AF6">
-        <v>0.0009938784695522982</v>
+        <v>0.0009605922108778969</v>
       </c>
       <c r="AG6">
-        <v>0.7316679138407259</v>
+        <v>0.8195197042551515</v>
       </c>
       <c r="AH6">
-        <v>884.8169753298216</v>
+        <v>843.49852971526</v>
       </c>
       <c r="AI6">
-        <v>0.000996522186913711</v>
+        <v>0.0009400872434948101</v>
       </c>
       <c r="AJ6">
-        <v>0.09289219499327084</v>
+        <v>0.09401617901571901</v>
       </c>
       <c r="AK6">
-        <v>8.737289720709475</v>
+        <v>6.717572957623268</v>
       </c>
       <c r="AL6">
-        <v>0.0009997890353576574</v>
+        <v>0.0009264203165137014</v>
       </c>
       <c r="AM6">
-        <v>0.6604266005937671</v>
+        <v>0.6725357237987079</v>
       </c>
       <c r="AN6">
-        <v>24.49978526467693</v>
+        <v>24.38596837934758</v>
       </c>
       <c r="AO6">
-        <v>0.0009628904602595457</v>
+        <v>0.001001363094425124</v>
       </c>
       <c r="AP6">
-        <v>0.7382846917338364</v>
+        <v>0.7301417836801415</v>
       </c>
       <c r="AQ6">
-        <v>124.103253809559</v>
+        <v>125.5822890087317</v>
       </c>
       <c r="AR6">
-        <v>0.0009876748495590065</v>
+        <v>0.00103845728802504</v>
       </c>
       <c r="AS6">
-        <v>1.544361436226974</v>
+        <v>1.517295693916493</v>
       </c>
       <c r="AT6">
-        <v>427.719890611368</v>
+        <v>389.736586751124</v>
       </c>
       <c r="AU6">
-        <v>0.00105060473426253</v>
+        <v>0.0009906462555755999</v>
       </c>
     </row>
     <row r="7" spans="1:47">
@@ -1375,7 +1375,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>50.4124976097772</v>
+        <v>43.62467083948572</v>
       </c>
       <c r="C7">
         <v>87.214</v>
@@ -1387,130 +1387,130 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>409.5818605352842</v>
+        <v>414.5514065133547</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>471.3465479702006</v>
+        <v>269.5634899355946</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.0115593701306427</v>
+        <v>0.01263230427499608</v>
       </c>
       <c r="K7">
-        <v>0.02163911850696281</v>
+        <v>0.01980856229327734</v>
       </c>
       <c r="L7">
-        <v>0.04834557376607278</v>
+        <v>0.0589489832372197</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>917.9267738720172</v>
+        <v>794.1410701593818</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>8.2053283320439</v>
+        <v>8.21098811116061</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>24.11055670237913</v>
+        <v>25.00946012993956</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7">
-        <v>123.3216869429173</v>
+        <v>135.6984850407951</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7">
-        <v>429.1411035744508</v>
+        <v>399.1702973901207</v>
       </c>
       <c r="W7">
-        <v>0.00103222837112759</v>
+        <v>0.001047984128462323</v>
       </c>
       <c r="X7">
-        <v>0.9207980289404357</v>
+        <v>0.9300716738316999</v>
       </c>
       <c r="Y7">
-        <v>1097.083050491956</v>
+        <v>1108.132116961173</v>
       </c>
       <c r="Z7">
-        <v>0.001001043092969317</v>
+        <v>0.0009754977379296209</v>
       </c>
       <c r="AA7">
-        <v>0.4841647870514185</v>
+        <v>0.5381098289691939</v>
       </c>
       <c r="AB7">
-        <v>198.3051142861897</v>
+        <v>223.0741864578401</v>
       </c>
       <c r="AC7">
-        <v>0.001036710928615358</v>
+        <v>0.0009971641546791404</v>
       </c>
       <c r="AD7">
-        <v>0.8337009617312289</v>
+        <v>0.8433603956271467</v>
       </c>
       <c r="AE7">
-        <v>392.9620703514511</v>
+        <v>227.3391715187174</v>
       </c>
       <c r="AF7">
-        <v>0.001026830021870312</v>
+        <v>0.0009789502001079618</v>
       </c>
       <c r="AG7">
-        <v>0.8184509838320568</v>
+        <v>0.7950741567882387</v>
       </c>
       <c r="AH7">
-        <v>917.9267738720172</v>
+        <v>794.1410701593818</v>
       </c>
       <c r="AI7">
-        <v>0.0009803846984571256</v>
+        <v>0.001002202479834981</v>
       </c>
       <c r="AJ7">
-        <v>0.08901977284343369</v>
+        <v>0.09314205828825697</v>
       </c>
       <c r="AK7">
-        <v>8.2053283320439</v>
+        <v>8.21098811116061</v>
       </c>
       <c r="AL7">
-        <v>0.0009980913003228525</v>
+        <v>0.0009601092263461838</v>
       </c>
       <c r="AM7">
-        <v>0.716255901702859</v>
+        <v>0.7035111206848927</v>
       </c>
       <c r="AN7">
-        <v>24.11055670237913</v>
+        <v>25.00946012993956</v>
       </c>
       <c r="AO7">
-        <v>0.000987222130449116</v>
+        <v>0.0009737907777969247</v>
       </c>
       <c r="AP7">
-        <v>0.7302720329152829</v>
+        <v>0.7407029435167009</v>
       </c>
       <c r="AQ7">
-        <v>123.3216869429173</v>
+        <v>135.6984850407951</v>
       </c>
       <c r="AR7">
-        <v>0.001015238521390537</v>
+        <v>0.001012812417568742</v>
       </c>
       <c r="AS7">
-        <v>1.577135207921025</v>
+        <v>1.578923154454077</v>
       </c>
       <c r="AT7">
-        <v>429.1411035744508</v>
+        <v>399.1702973901207</v>
       </c>
       <c r="AU7">
-        <v>0.00101825318391506</v>
+        <v>0.0009753166434036829</v>
       </c>
     </row>
     <row r="8" spans="1:47">
@@ -1518,7 +1518,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>46.45343351146381</v>
+        <v>45.20985617486821</v>
       </c>
       <c r="C8">
         <v>87.214</v>
@@ -1530,130 +1530,130 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>350.7962705846295</v>
+        <v>401.2805919057457</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>419.8405419433377</v>
+        <v>405.4892705981244</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.01221500726326247</v>
+        <v>0.01198449688344554</v>
       </c>
       <c r="K8">
-        <v>0.02225055158943944</v>
+        <v>0.01887316264742945</v>
       </c>
       <c r="L8">
-        <v>0.0462890681434457</v>
+        <v>0.04609960385625889</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>884.2651544565878</v>
+        <v>849.1633344188325</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>7.327071177271991</v>
+        <v>8.272210180114422</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>21.10474558090227</v>
+        <v>20.6764595173407</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8">
-        <v>128.4723966786975</v>
+        <v>136.8452643832534</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8">
-        <v>383.2247935236371</v>
+        <v>400.4068609255361</v>
       </c>
       <c r="W8">
-        <v>0.0009959700921338538</v>
+        <v>0.0009898984385455396</v>
       </c>
       <c r="X8">
-        <v>0.9278107947714941</v>
+        <v>0.9270223623041723</v>
       </c>
       <c r="Y8">
-        <v>1105.438396928977</v>
+        <v>1104.499020573717</v>
       </c>
       <c r="Z8">
-        <v>0.0009690644202666475</v>
+        <v>0.001014791184466741</v>
       </c>
       <c r="AA8">
-        <v>0.5355568728510918</v>
+        <v>0.5772899405150905</v>
       </c>
       <c r="AB8">
-        <v>187.8713536821296</v>
+        <v>231.6552490311283</v>
       </c>
       <c r="AC8">
-        <v>0.001041679754516661</v>
+        <v>0.000970504997651254</v>
       </c>
       <c r="AD8">
-        <v>0.8302377890837584</v>
+        <v>0.8398781000580512</v>
       </c>
       <c r="AE8">
-        <v>348.5674833107637</v>
+        <v>340.5615581838779</v>
       </c>
       <c r="AF8">
-        <v>0.0009877800162896933</v>
+        <v>0.0009503681883667623</v>
       </c>
       <c r="AG8">
-        <v>0.8024545302063717</v>
+        <v>0.7678928619409277</v>
       </c>
       <c r="AH8">
-        <v>884.2651544565878</v>
+        <v>849.1633344188325</v>
       </c>
       <c r="AI8">
-        <v>0.0009729316292056278</v>
+        <v>0.000995102869296615</v>
       </c>
       <c r="AJ8">
-        <v>0.08902574731289617</v>
+        <v>0.09132432038137561</v>
       </c>
       <c r="AK8">
-        <v>7.327071177271991</v>
+        <v>8.272210180114422</v>
       </c>
       <c r="AL8">
-        <v>0.0010015735249383</v>
+        <v>0.00102640745005034</v>
       </c>
       <c r="AM8">
-        <v>0.6799211049065302</v>
+        <v>0.7298543760698564</v>
       </c>
       <c r="AN8">
-        <v>21.10474558090227</v>
+        <v>20.6764595173407</v>
       </c>
       <c r="AO8">
-        <v>0.000945519194165645</v>
+        <v>0.0009959641769313016</v>
       </c>
       <c r="AP8">
-        <v>0.7287254523378432</v>
+        <v>0.7057141017273874</v>
       </c>
       <c r="AQ8">
-        <v>128.4723966786975</v>
+        <v>136.8452643832534</v>
       </c>
       <c r="AR8">
-        <v>0.0009646180035735486</v>
+        <v>0.0009579716768094207</v>
       </c>
       <c r="AS8">
-        <v>1.531144250857656</v>
+        <v>1.551605903306142</v>
       </c>
       <c r="AT8">
-        <v>383.2247935236371</v>
+        <v>400.4068609255361</v>
       </c>
       <c r="AU8">
-        <v>0.0009875555572686173</v>
+        <v>0.0009836717566938178</v>
       </c>
     </row>
     <row r="9" spans="1:47">
@@ -1661,7 +1661,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>43.1678687659523</v>
+        <v>36.52163372700973</v>
       </c>
       <c r="C9">
         <v>87.214</v>
@@ -1673,130 +1673,130 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>414.5798653905349</v>
+        <v>376.9832239944132</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>291.5735845143979</v>
+        <v>238.9860576494445</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.01453898486051059</v>
+        <v>0.01120297084013906</v>
       </c>
       <c r="K9">
-        <v>0.01994919400983459</v>
+        <v>0.02051498613465822</v>
       </c>
       <c r="L9">
-        <v>0.04460635802978818</v>
+        <v>0.04603741285602544</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>797.8140895642164</v>
+        <v>729.720435521269</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>7.819099399464234</v>
+        <v>6.53284363416182</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9">
-        <v>24.43298978232311</v>
+        <v>23.49765524195348</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9">
-        <v>131.5739553402753</v>
+        <v>135.5804200905612</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9">
-        <v>397.156044923588</v>
+        <v>437.9606077372964</v>
       </c>
       <c r="W9">
-        <v>0.0009565922334546941</v>
+        <v>0.001024221469438774</v>
       </c>
       <c r="X9">
-        <v>0.9215630036300078</v>
+        <v>0.9302782533079506</v>
       </c>
       <c r="Y9">
-        <v>1097.99447812278</v>
+        <v>1108.378245683055</v>
       </c>
       <c r="Z9">
-        <v>0.001086250714541437</v>
+        <v>0.0009918497778098239</v>
       </c>
       <c r="AA9">
-        <v>0.5691105711208442</v>
+        <v>0.561806314322566</v>
       </c>
       <c r="AB9">
-        <v>235.94178396761</v>
+        <v>211.7915556337396</v>
       </c>
       <c r="AC9">
-        <v>0.001009631254762037</v>
+        <v>0.001022987271771219</v>
       </c>
       <c r="AD9">
-        <v>0.8441821924044465</v>
+        <v>0.8465921602690555</v>
       </c>
       <c r="AE9">
-        <v>246.1412278225876</v>
+        <v>202.3237228196283</v>
       </c>
       <c r="AF9">
-        <v>0.001086302496064317</v>
+        <v>0.001014385450150446</v>
       </c>
       <c r="AG9">
-        <v>0.7895338032710291</v>
+        <v>0.7711097166602339</v>
       </c>
       <c r="AH9">
-        <v>797.8140895642164</v>
+        <v>729.720435521269</v>
       </c>
       <c r="AI9">
-        <v>0.001009218541712742</v>
+        <v>0.0009530212880277476</v>
       </c>
       <c r="AJ9">
-        <v>0.08504939119592506</v>
+        <v>0.09300378065756107</v>
       </c>
       <c r="AK9">
-        <v>7.819099399464234</v>
+        <v>6.53284363416182</v>
       </c>
       <c r="AL9">
-        <v>0.001011517736352169</v>
+        <v>0.0009980340671248084</v>
       </c>
       <c r="AM9">
-        <v>0.7259146105538943</v>
+        <v>0.7252099797777273</v>
       </c>
       <c r="AN9">
-        <v>24.43298978232311</v>
+        <v>23.49765524195348</v>
       </c>
       <c r="AO9">
-        <v>0.0009265411210371266</v>
+        <v>0.001013096211114973</v>
       </c>
       <c r="AP9">
-        <v>0.6906643365657243</v>
+        <v>0.7164691018568082</v>
       </c>
       <c r="AQ9">
-        <v>131.5739553402753</v>
+        <v>135.5804200905612</v>
       </c>
       <c r="AR9">
-        <v>0.001005630224960974</v>
+        <v>0.001010889202405906</v>
       </c>
       <c r="AS9">
-        <v>1.566738384420754</v>
+        <v>1.540539647914184</v>
       </c>
       <c r="AT9">
-        <v>397.156044923588</v>
+        <v>437.9606077372964</v>
       </c>
       <c r="AU9">
-        <v>0.001008268632453157</v>
+        <v>0.001008558958148596</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -1804,7 +1804,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>49.46994593577116</v>
+        <v>46.66520725823986</v>
       </c>
       <c r="C10">
         <v>87.214</v>
@@ -1816,130 +1816,130 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>397.9381610577143</v>
+        <v>427.1954927925835</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>462.6520399337339</v>
+        <v>368.2578060247981</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.01067197562494157</v>
+        <v>0.01298746097883421</v>
       </c>
       <c r="K10">
-        <v>0.02003579250836286</v>
+        <v>0.02041887850393756</v>
       </c>
       <c r="L10">
-        <v>0.05185975503842222</v>
+        <v>0.04766394190427051</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>886.2451561473425</v>
+        <v>827.201081257007</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>6.830469412716987</v>
+        <v>7.011025699076625</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>25.45742625549875</v>
+        <v>24.64489214498487</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10">
-        <v>120.1540015677081</v>
+        <v>142.1529484748365</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10">
-        <v>441.2598853030874</v>
+        <v>421.9749589719078</v>
       </c>
       <c r="W10">
-        <v>0.0009781476248998666</v>
+        <v>0.001084144884237837</v>
       </c>
       <c r="X10">
-        <v>0.9266022660683876</v>
+        <v>0.936741425049466</v>
       </c>
       <c r="Y10">
-        <v>1103.998497717054</v>
+        <v>1116.078779293226</v>
       </c>
       <c r="Z10">
-        <v>0.0009538419395478099</v>
+        <v>0.0009439755732867818</v>
       </c>
       <c r="AA10">
-        <v>0.5125286049493564</v>
+        <v>0.5618184121905332</v>
       </c>
       <c r="AB10">
-        <v>203.9546905430226</v>
+        <v>240.0062934556816</v>
       </c>
       <c r="AC10">
-        <v>0.001032562442448242</v>
+        <v>0.001042851199780057</v>
       </c>
       <c r="AD10">
-        <v>0.8428890224806687</v>
+        <v>0.8269352650827787</v>
       </c>
       <c r="AE10">
-        <v>389.9643256884324</v>
+        <v>304.525366443919</v>
       </c>
       <c r="AF10">
-        <v>0.0009549572518032436</v>
+        <v>0.001054129801543454</v>
       </c>
       <c r="AG10">
-        <v>0.7880934930243833</v>
+        <v>0.7779654613075666</v>
       </c>
       <c r="AH10">
-        <v>886.2451561473425</v>
+        <v>827.201081257007</v>
       </c>
       <c r="AI10">
-        <v>0.001018114626745048</v>
+        <v>0.0009931788741499171</v>
       </c>
       <c r="AJ10">
-        <v>0.08714104607987097</v>
+        <v>0.09171624854755538</v>
       </c>
       <c r="AK10">
-        <v>6.830469412716987</v>
+        <v>7.011025699076625</v>
       </c>
       <c r="AL10">
-        <v>0.0009855731388378436</v>
+        <v>0.0009678550680619972</v>
       </c>
       <c r="AM10">
-        <v>0.6940252081989126</v>
+        <v>0.7066007829173676</v>
       </c>
       <c r="AN10">
-        <v>25.45742625549875</v>
+        <v>24.64489214498487</v>
       </c>
       <c r="AO10">
-        <v>0.001019314639657623</v>
+        <v>0.0009811649784716118</v>
       </c>
       <c r="AP10">
-        <v>0.6862333820279769</v>
+        <v>0.684793827183523</v>
       </c>
       <c r="AQ10">
-        <v>120.1540015677081</v>
+        <v>142.1529484748365</v>
       </c>
       <c r="AR10">
-        <v>0.0009889039540701909</v>
+        <v>0.001020393686470805</v>
       </c>
       <c r="AS10">
-        <v>1.55802533132158</v>
+        <v>1.515621718652084</v>
       </c>
       <c r="AT10">
-        <v>441.2598853030874</v>
+        <v>421.9749589719078</v>
       </c>
       <c r="AU10">
-        <v>0.0009862243328073225</v>
+        <v>0.00101702063279151</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -1947,7 +1947,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44.0183610008897</v>
+        <v>48.81317497871006</v>
       </c>
       <c r="C11">
         <v>87.214</v>
@@ -1959,130 +1959,130 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>386.1220110217505</v>
+        <v>405.2634899343079</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>348.7806586884058</v>
+        <v>382.0792416647751</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.01158456969326583</v>
+        <v>0.01162395510564761</v>
       </c>
       <c r="K11">
-        <v>0.01597559821144815</v>
+        <v>0.02151426118769679</v>
       </c>
       <c r="L11">
-        <v>0.05568294592094519</v>
+        <v>0.05641738525872021</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>822.9484112648463</v>
+        <v>866.3499903959437</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11">
-        <v>9.096424350780993</v>
+        <v>8.678295830319616</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11">
-        <v>23.12175279582004</v>
+        <v>24.48889183574896</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
-        <v>121.7366781215214</v>
+        <v>120.9024851130247</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11">
-        <v>412.371546636754</v>
+        <v>418.005784477503</v>
       </c>
       <c r="W11">
-        <v>0.001035316271429</v>
+        <v>0.0009274138871512964</v>
       </c>
       <c r="X11">
-        <v>0.9154212817047211</v>
+        <v>0.9347102686345224</v>
       </c>
       <c r="Y11">
-        <v>1090.67693528136</v>
+        <v>1113.658761867367</v>
       </c>
       <c r="Z11">
-        <v>0.0009551027213642876</v>
+        <v>0.001030076216368467</v>
       </c>
       <c r="AA11">
-        <v>0.5772583923175891</v>
+        <v>0.5627821963369624</v>
       </c>
       <c r="AB11">
-        <v>222.8921713208501</v>
+        <v>228.0750769604122</v>
       </c>
       <c r="AC11">
-        <v>0.001040226781289399</v>
+        <v>0.00103437175606057</v>
       </c>
       <c r="AD11">
-        <v>0.8546242323962552</v>
+        <v>0.842734907407205</v>
       </c>
       <c r="AE11">
-        <v>298.0764027062392</v>
+        <v>321.9915143465794</v>
       </c>
       <c r="AF11">
-        <v>0.0009728302067622544</v>
+        <v>0.0009468652747151984</v>
       </c>
       <c r="AG11">
-        <v>0.7919740011160821</v>
+        <v>0.7954438089835503</v>
       </c>
       <c r="AH11">
-        <v>822.9484112648463</v>
+        <v>866.3499903959437</v>
       </c>
       <c r="AI11">
-        <v>0.001047939325548917</v>
+        <v>0.0009501158914993185</v>
       </c>
       <c r="AJ11">
-        <v>0.09128877806844127</v>
+        <v>0.08751077886526835</v>
       </c>
       <c r="AK11">
-        <v>9.096424350780993</v>
+        <v>8.678295830319616</v>
       </c>
       <c r="AL11">
-        <v>0.0009479942449879079</v>
+        <v>0.001003674187104192</v>
       </c>
       <c r="AM11">
-        <v>0.675668254362135</v>
+        <v>0.6615597097098642</v>
       </c>
       <c r="AN11">
-        <v>23.12175279582004</v>
+        <v>24.48889183574896</v>
       </c>
       <c r="AO11">
-        <v>0.001053460839844618</v>
+        <v>0.001006603968753571</v>
       </c>
       <c r="AP11">
-        <v>0.7230218043233839</v>
+        <v>0.7395801543366415</v>
       </c>
       <c r="AQ11">
-        <v>121.7366781215214</v>
+        <v>120.9024851130247</v>
       </c>
       <c r="AR11">
-        <v>0.001039378478280553</v>
+        <v>0.001053644437299344</v>
       </c>
       <c r="AS11">
-        <v>1.525618281206616</v>
+        <v>1.520434292408784</v>
       </c>
       <c r="AT11">
-        <v>412.371546636754</v>
+        <v>418.005784477503</v>
       </c>
       <c r="AU11">
-        <v>0.0009836155480028889</v>
+        <v>0.001005509676303631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>